<commit_message>
Fix naming of with/without trap
</commit_message>
<xml_diff>
--- a/inst/scripts/examples/trap_example/example_with_trap.xlsx
+++ b/inst/scripts/examples/trap_example/example_with_trap.xlsx
@@ -880,7 +880,9 @@
       <c r="H5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="I5" s="18"/>
+      <c r="I5" s="18">
+        <v>-1.0</v>
+      </c>
       <c r="J5" s="15"/>
       <c r="K5" s="16"/>
       <c r="L5" s="1"/>

</xml_diff>